<commit_message>
add auto report examples
</commit_message>
<xml_diff>
--- a/examples/model_report/三方数据测试报告.xlsx
+++ b/examples/model_report/三方数据测试报告.xlsx
@@ -1559,7 +1559,7 @@
     <row r="14">
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>特征: duration_in_month</t>
+          <t>数据字段: duration_in_month</t>
         </is>
       </c>
       <c r="C14" s="3" t="n"/>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="C37" s="11" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D37" s="11" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="C38" s="13" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D38" s="13" t="inlineStr">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="C39" s="11" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D39" s="11" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="C40" s="13" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D40" s="13" t="inlineStr">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="C41" s="11" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D41" s="11" t="inlineStr">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="C42" s="13" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D42" s="13" t="inlineStr">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="C43" s="11" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D43" s="11" t="inlineStr">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="C44" s="13" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D44" s="13" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="C45" s="11" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D45" s="11" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C46" s="15" t="inlineStr">
         <is>
-          <t>duration_in_month 评分效果</t>
+          <t>duration_in_month</t>
         </is>
       </c>
       <c r="D46" s="15" t="inlineStr">
@@ -2295,7 +2295,7 @@
     <row r="49">
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>特征: credit_amount</t>
+          <t>数据字段: credit_amount</t>
         </is>
       </c>
       <c r="C49" s="3" t="n"/>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C72" s="11" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D72" s="11" t="inlineStr">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="C73" s="13" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D73" s="13" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="C74" s="11" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D74" s="11" t="inlineStr">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="C75" s="13" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D75" s="13" t="inlineStr">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="C76" s="11" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D76" s="11" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="C77" s="13" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D77" s="13" t="inlineStr">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="C78" s="11" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D78" s="11" t="inlineStr">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="C79" s="13" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D79" s="13" t="inlineStr">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="C80" s="11" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D80" s="11" t="inlineStr">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="C81" s="15" t="inlineStr">
         <is>
-          <t>credit_amount 评分效果</t>
+          <t>credit_amount</t>
         </is>
       </c>
       <c r="D81" s="15" t="inlineStr">
@@ -3031,7 +3031,7 @@
     <row r="84">
       <c r="B84" s="5" t="inlineStr">
         <is>
-          <t>特征: installment_rate_in_percentage_of_disposable_income</t>
+          <t>数据字段: installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="C84" s="3" t="n"/>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="C107" s="11" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D107" s="11" t="inlineStr">
@@ -3214,7 +3214,7 @@
       </c>
       <c r="C108" s="13" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D108" s="13" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="C109" s="11" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D109" s="11" t="inlineStr">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="C110" s="13" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D110" s="13" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="C111" s="11" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D111" s="11" t="inlineStr">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="C112" s="13" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D112" s="13" t="inlineStr">
@@ -3524,7 +3524,7 @@
       </c>
       <c r="C113" s="11" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D113" s="11" t="inlineStr">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="C114" s="13" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D114" s="13" t="inlineStr">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="C115" s="11" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D115" s="11" t="inlineStr">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="C116" s="15" t="inlineStr">
         <is>
-          <t>installment_rate_in_percentage_of_disposable_income 评分效果</t>
+          <t>installment_rate_in_percentage_of_disposable_income</t>
         </is>
       </c>
       <c r="D116" s="15" t="inlineStr">
@@ -3767,7 +3767,7 @@
     <row r="119">
       <c r="B119" s="5" t="inlineStr">
         <is>
-          <t>特征: present_residence_since</t>
+          <t>数据字段: present_residence_since</t>
         </is>
       </c>
       <c r="C119" s="3" t="n"/>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="C142" s="11" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D142" s="11" t="inlineStr">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="C143" s="13" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D143" s="13" t="inlineStr">
@@ -4012,7 +4012,7 @@
       </c>
       <c r="C144" s="11" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D144" s="11" t="inlineStr">
@@ -4074,7 +4074,7 @@
       </c>
       <c r="C145" s="13" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D145" s="13" t="inlineStr">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="C146" s="11" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D146" s="11" t="inlineStr">
@@ -4198,7 +4198,7 @@
       </c>
       <c r="C147" s="13" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D147" s="13" t="inlineStr">
@@ -4260,7 +4260,7 @@
       </c>
       <c r="C148" s="11" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D148" s="11" t="inlineStr">
@@ -4322,7 +4322,7 @@
       </c>
       <c r="C149" s="13" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D149" s="13" t="inlineStr">
@@ -4384,7 +4384,7 @@
       </c>
       <c r="C150" s="11" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D150" s="11" t="inlineStr">
@@ -4446,7 +4446,7 @@
       </c>
       <c r="C151" s="15" t="inlineStr">
         <is>
-          <t>present_residence_since 评分效果</t>
+          <t>present_residence_since</t>
         </is>
       </c>
       <c r="D151" s="15" t="inlineStr">
@@ -4503,7 +4503,7 @@
     <row r="154">
       <c r="B154" s="5" t="inlineStr">
         <is>
-          <t>特征: age_in_years</t>
+          <t>数据字段: age_in_years</t>
         </is>
       </c>
       <c r="C154" s="3" t="n"/>
@@ -4624,7 +4624,7 @@
       </c>
       <c r="C177" s="11" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D177" s="11" t="inlineStr">
@@ -4686,7 +4686,7 @@
       </c>
       <c r="C178" s="13" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D178" s="13" t="inlineStr">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C179" s="11" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D179" s="11" t="inlineStr">
@@ -4810,7 +4810,7 @@
       </c>
       <c r="C180" s="13" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D180" s="13" t="inlineStr">
@@ -4872,7 +4872,7 @@
       </c>
       <c r="C181" s="11" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D181" s="11" t="inlineStr">
@@ -4934,7 +4934,7 @@
       </c>
       <c r="C182" s="13" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D182" s="13" t="inlineStr">
@@ -4996,7 +4996,7 @@
       </c>
       <c r="C183" s="11" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D183" s="11" t="inlineStr">
@@ -5058,7 +5058,7 @@
       </c>
       <c r="C184" s="13" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D184" s="13" t="inlineStr">
@@ -5120,7 +5120,7 @@
       </c>
       <c r="C185" s="11" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D185" s="11" t="inlineStr">
@@ -5182,7 +5182,7 @@
       </c>
       <c r="C186" s="15" t="inlineStr">
         <is>
-          <t>age_in_years 评分效果</t>
+          <t>age_in_years</t>
         </is>
       </c>
       <c r="D186" s="15" t="inlineStr">
@@ -5239,7 +5239,7 @@
     <row r="189">
       <c r="B189" s="5" t="inlineStr">
         <is>
-          <t>特征: number_of_existing_credits_at_this_bank</t>
+          <t>数据字段: number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="C189" s="3" t="n"/>
@@ -5360,7 +5360,7 @@
       </c>
       <c r="C212" s="11" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D212" s="11" t="inlineStr">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C213" s="13" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D213" s="13" t="inlineStr">
@@ -5484,7 +5484,7 @@
       </c>
       <c r="C214" s="11" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D214" s="11" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="C215" s="13" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D215" s="13" t="inlineStr">
@@ -5608,7 +5608,7 @@
       </c>
       <c r="C216" s="11" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D216" s="11" t="inlineStr">
@@ -5670,7 +5670,7 @@
       </c>
       <c r="C217" s="13" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D217" s="13" t="inlineStr">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="C218" s="11" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D218" s="11" t="inlineStr">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="C219" s="13" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D219" s="13" t="inlineStr">
@@ -5856,7 +5856,7 @@
       </c>
       <c r="C220" s="11" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D220" s="11" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="C221" s="15" t="inlineStr">
         <is>
-          <t>number_of_existing_credits_at_this_bank 评分效果</t>
+          <t>number_of_existing_credits_at_this_bank</t>
         </is>
       </c>
       <c r="D221" s="15" t="inlineStr">
@@ -5975,7 +5975,7 @@
     <row r="224">
       <c r="B224" s="5" t="inlineStr">
         <is>
-          <t>特征: number_of_people_being_liable_to_provide_maintenance_for</t>
+          <t>数据字段: number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="C224" s="3" t="n"/>
@@ -6096,7 +6096,7 @@
       </c>
       <c r="C247" s="11" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D247" s="11" t="inlineStr">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="C248" s="13" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D248" s="13" t="inlineStr">
@@ -6220,7 +6220,7 @@
       </c>
       <c r="C249" s="11" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D249" s="11" t="inlineStr">
@@ -6282,7 +6282,7 @@
       </c>
       <c r="C250" s="13" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D250" s="13" t="inlineStr">
@@ -6344,7 +6344,7 @@
       </c>
       <c r="C251" s="11" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D251" s="11" t="inlineStr">
@@ -6406,7 +6406,7 @@
       </c>
       <c r="C252" s="13" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D252" s="13" t="inlineStr">
@@ -6468,7 +6468,7 @@
       </c>
       <c r="C253" s="11" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D253" s="11" t="inlineStr">
@@ -6530,7 +6530,7 @@
       </c>
       <c r="C254" s="13" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D254" s="13" t="inlineStr">
@@ -6592,7 +6592,7 @@
       </c>
       <c r="C255" s="11" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D255" s="11" t="inlineStr">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="C256" s="15" t="inlineStr">
         <is>
-          <t>number_of_people_being_liable_to_provide_maintenance_for 评分效果</t>
+          <t>number_of_people_being_liable_to_provide_maintenance_for</t>
         </is>
       </c>
       <c r="D256" s="15" t="inlineStr">

</xml_diff>